<commit_message>
db tables + question type 0 implemented
</commit_message>
<xml_diff>
--- a/public/txt&csv/db table/Q1type.xlsx
+++ b/public/txt&csv/db table/Q1type.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>drinkingIssuesExtraLargeHierCC.xgml</t>
   </si>
@@ -246,6 +246,45 @@
   </si>
   <si>
     <t>meditation</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>domain_name</t>
+  </si>
+  <si>
+    <t>node-link</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>hier</t>
+  </si>
+  <si>
+    <t>drinking</t>
+  </si>
+  <si>
+    <t>organic</t>
+  </si>
+  <si>
+    <t>radial</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>student</t>
   </si>
 </sst>
 </file>
@@ -597,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +647,11 @@
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -623,8 +664,20 @@
       <c r="D1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -637,8 +690,20 @@
       <c r="D2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -651,8 +716,20 @@
       <c r="D3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -665,8 +742,20 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -676,8 +765,20 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -690,8 +791,20 @@
       <c r="D6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -704,8 +817,20 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -718,8 +843,20 @@
       <c r="D8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -732,8 +869,20 @@
       <c r="D9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -746,8 +895,20 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -760,8 +921,20 @@
       <c r="D11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -774,8 +947,20 @@
       <c r="D12" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -788,8 +973,20 @@
       <c r="D13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -802,8 +999,20 @@
       <c r="D14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -816,8 +1025,20 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -830,8 +1051,20 @@
       <c r="D16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -841,8 +1074,20 @@
       <c r="D17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -855,8 +1100,20 @@
       <c r="D18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -868,6 +1125,18 @@
       </c>
       <c r="D19" t="s">
         <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>